<commit_message>
Refactor Amdo & Erythyro - add flanking genes, adjust orthology
</commit_message>
<xml_diff>
--- a/tabular/eve/parvovirinae/epv-amdo-side-data.xlsx
+++ b/tabular/eve/parvovirinae/epv-amdo-side-data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/Parvoviridae-GLUE/tabular/eve/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/Parvoviridae-GLUE/tabular/eve/parvovirinae/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1733C57-D985-EF4D-9400-2442D3205EB3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B631DEEE-3BC7-6949-B400-9BCFEC1DD90D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19720" yWindow="2720" windowWidth="31140" windowHeight="26000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11400" yWindow="5040" windowWidth="31140" windowHeight="26000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="query_result" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="105">
   <si>
     <t>host_species</t>
   </si>
@@ -217,9 +217,6 @@
     <t>scaffold_34481</t>
   </si>
   <si>
-    <t>ap.102-procavia</t>
-  </si>
-  <si>
     <t>Heterohyrax_brucei</t>
   </si>
   <si>
@@ -325,10 +322,19 @@
     <t>ap.101-Protobothrops_mucrosquamatus</t>
   </si>
   <si>
-    <t>ap.101-Ptyas_mucosa</t>
-  </si>
-  <si>
     <t>ap.101-serpentes-UR</t>
+  </si>
+  <si>
+    <t>ap.105-Ptyas_mucosa</t>
+  </si>
+  <si>
+    <t>ap.105-ptyas</t>
+  </si>
+  <si>
+    <t>ap.102-hyracoidae</t>
+  </si>
+  <si>
+    <t>ap.105</t>
   </si>
 </sst>
 </file>
@@ -479,7 +485,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -668,6 +674,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59996337778862885"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -832,19 +850,20 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1202,8 +1221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
-      <selection sqref="A1:AE10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1216,959 +1235,958 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="A1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="U1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="V1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="W1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="X1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Y1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="Z1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AA1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AB1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AC1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AD1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AE1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="5">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D2" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="4">
         <v>4462</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="4">
         <v>10041</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="4">
         <v>598</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="4">
         <v>1305</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="4">
         <v>1859</v>
       </c>
-      <c r="Q2">
+      <c r="Q2" s="4">
         <v>3982</v>
       </c>
-      <c r="R2">
+      <c r="R2" s="4">
         <v>708</v>
       </c>
-      <c r="S2">
+      <c r="S2" s="4">
         <v>1372</v>
       </c>
-      <c r="T2">
+      <c r="T2" s="4">
         <v>100</v>
       </c>
-      <c r="U2">
+      <c r="U2" s="4">
         <v>0</v>
       </c>
-      <c r="V2">
+      <c r="V2" s="4">
         <v>1</v>
       </c>
-      <c r="W2">
+      <c r="W2" s="4">
         <v>0</v>
       </c>
-      <c r="X2">
+      <c r="X2" s="4">
         <v>0</v>
       </c>
-      <c r="Y2">
+      <c r="Y2" s="4">
         <v>5580</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="Z2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AA2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AB2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AC2" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AD2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AE2" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="A3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="5">
         <v>2</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D3" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="4">
         <v>110876</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="4">
         <v>112702</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="4">
         <v>3</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="4">
         <v>598</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="4">
         <v>1</v>
       </c>
-      <c r="Q3">
+      <c r="Q3" s="4">
         <v>1788</v>
       </c>
-      <c r="R3">
+      <c r="R3" s="4">
         <v>596</v>
       </c>
-      <c r="S3">
+      <c r="S3" s="4">
         <v>1230</v>
       </c>
-      <c r="T3">
+      <c r="T3" s="4">
         <v>100</v>
       </c>
-      <c r="U3">
+      <c r="U3" s="4">
         <v>0</v>
       </c>
-      <c r="V3">
+      <c r="V3" s="4">
         <v>1</v>
       </c>
-      <c r="W3">
+      <c r="W3" s="4">
         <v>0</v>
       </c>
-      <c r="X3">
+      <c r="X3" s="4">
         <v>0</v>
       </c>
-      <c r="Y3">
+      <c r="Y3" s="4">
         <v>1827</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="Z3" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AA3" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AB3" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AC3" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AD3" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AE3" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" s="5">
+        <v>101</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C4" s="4">
-        <v>101</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="E4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="4">
         <v>524</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="4">
         <v>853</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="4">
         <v>58</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="4">
         <v>167</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="4">
         <v>1</v>
       </c>
-      <c r="Q4">
+      <c r="Q4" s="4">
         <v>330</v>
       </c>
-      <c r="R4">
+      <c r="R4" s="4">
         <v>110</v>
       </c>
-      <c r="S4">
+      <c r="S4" s="4">
         <v>228</v>
       </c>
-      <c r="T4">
+      <c r="T4" s="4">
         <v>98.182000000000002</v>
       </c>
-      <c r="U4">
+      <c r="U4" s="4">
         <v>1.17</v>
       </c>
-      <c r="V4">
+      <c r="V4" s="4">
         <v>72</v>
       </c>
-      <c r="W4">
+      <c r="W4" s="4">
         <v>0</v>
       </c>
-      <c r="X4">
+      <c r="X4" s="4">
         <v>0</v>
       </c>
-      <c r="Y4">
+      <c r="Y4" s="4">
         <v>330</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="Z4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AA4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AB4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AC4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AD4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AE4" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B5" t="s">
-        <v>102</v>
-      </c>
-      <c r="C5" s="4">
+      <c r="A5" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" s="5">
         <v>101</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="D5" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="F5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="H5" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="I5" t="s">
-        <v>74</v>
-      </c>
-      <c r="J5" t="s">
+      <c r="J5" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="4">
         <v>115621</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="4">
         <v>115950</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="4">
         <v>58</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="4">
         <v>167</v>
       </c>
-      <c r="P5">
+      <c r="P5" s="4">
         <v>1</v>
       </c>
-      <c r="Q5">
+      <c r="Q5" s="4">
         <v>330</v>
       </c>
-      <c r="R5">
+      <c r="R5" s="4">
         <v>110</v>
       </c>
-      <c r="S5">
+      <c r="S5" s="4">
         <v>228</v>
       </c>
-      <c r="T5">
+      <c r="T5" s="4">
         <v>97.272999999999996</v>
       </c>
-      <c r="U5">
+      <c r="U5" s="4">
         <v>1.42</v>
       </c>
-      <c r="V5">
+      <c r="V5" s="4">
         <v>72</v>
       </c>
-      <c r="W5">
+      <c r="W5" s="4">
         <v>0</v>
       </c>
-      <c r="X5">
+      <c r="X5" s="4">
         <v>0</v>
       </c>
-      <c r="Y5">
+      <c r="Y5" s="4">
         <v>330</v>
       </c>
-      <c r="Z5" t="s">
-        <v>71</v>
-      </c>
-      <c r="AA5" t="s">
+      <c r="Z5" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="AB5" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="AC5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AD5" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AE5" t="s">
+      <c r="AE5" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B6" t="s">
-        <v>102</v>
-      </c>
-      <c r="C6" s="4">
+      <c r="A6" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="5">
         <v>101</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="D6" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="F6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="H6" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="I6" t="s">
-        <v>78</v>
-      </c>
-      <c r="J6" t="s">
+      <c r="J6" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="4">
         <v>1053444</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="4">
         <v>1057106</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="4">
         <v>401</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="4">
         <v>1003</v>
       </c>
-      <c r="P6">
+      <c r="P6" s="4">
         <v>1046</v>
       </c>
-      <c r="Q6">
+      <c r="Q6" s="4">
         <v>2815</v>
       </c>
-      <c r="R6">
+      <c r="R6" s="4">
         <v>609</v>
       </c>
-      <c r="S6">
+      <c r="S6" s="4">
         <v>934</v>
       </c>
-      <c r="T6">
+      <c r="T6" s="4">
         <v>84.400999999999996</v>
       </c>
-      <c r="U6">
+      <c r="U6" s="4">
         <v>0</v>
       </c>
-      <c r="V6">
+      <c r="V6" s="4">
         <v>1</v>
       </c>
-      <c r="W6">
+      <c r="W6" s="4">
         <v>5</v>
       </c>
-      <c r="X6">
+      <c r="X6" s="4">
         <v>0</v>
       </c>
-      <c r="Y6">
+      <c r="Y6" s="4">
         <v>3663</v>
       </c>
-      <c r="Z6" t="s">
-        <v>75</v>
-      </c>
-      <c r="AA6" t="s">
+      <c r="Z6" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AB6" t="s">
+      <c r="AB6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="AC6" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AD6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AE6" t="s">
+      <c r="AE6" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B7" t="s">
-        <v>102</v>
-      </c>
-      <c r="C7" s="4">
+      <c r="C7" s="5">
         <v>101</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="D7" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="4">
         <v>97680</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="4">
         <v>101695</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="4">
         <v>1</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="4">
         <v>487</v>
       </c>
-      <c r="P7">
+      <c r="P7" s="4">
         <v>1</v>
       </c>
-      <c r="Q7">
+      <c r="Q7" s="4">
         <v>1461</v>
       </c>
-      <c r="R7">
+      <c r="R7" s="4">
         <v>487</v>
       </c>
-      <c r="S7">
+      <c r="S7" s="4">
         <v>858</v>
       </c>
-      <c r="T7">
+      <c r="T7" s="4">
         <v>97.947000000000003</v>
       </c>
-      <c r="U7">
+      <c r="U7" s="4">
         <v>0</v>
       </c>
-      <c r="V7">
+      <c r="V7" s="4">
         <v>1</v>
       </c>
-      <c r="W7">
+      <c r="W7" s="4">
         <v>0</v>
       </c>
-      <c r="X7">
+      <c r="X7" s="4">
         <v>0</v>
       </c>
-      <c r="Y7">
+      <c r="Y7" s="4">
         <v>4016</v>
       </c>
-      <c r="Z7" t="s">
+      <c r="Z7" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AA7" t="s">
+      <c r="AA7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AB7" t="s">
+      <c r="AB7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AC7" t="s">
+      <c r="AC7" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AD7" t="s">
+      <c r="AD7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AE7" t="s">
+      <c r="AE7" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="A8" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8" s="5">
         <v>102</v>
       </c>
-      <c r="C8" s="4">
-        <v>101</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="K8" s="4">
+        <v>8211</v>
+      </c>
+      <c r="L8" s="4">
+        <v>8465</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="N8" s="4">
+        <v>14</v>
+      </c>
+      <c r="O8" s="4">
         <v>97</v>
       </c>
-      <c r="E8" t="s">
-        <v>79</v>
-      </c>
-      <c r="F8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" t="s">
-        <v>82</v>
-      </c>
-      <c r="H8" t="s">
-        <v>83</v>
-      </c>
-      <c r="I8" t="s">
+      <c r="P8" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="4">
+        <v>252</v>
+      </c>
+      <c r="R8" s="4">
         <v>84</v>
       </c>
-      <c r="J8" t="s">
-        <v>37</v>
-      </c>
-      <c r="K8">
-        <v>8651751</v>
-      </c>
-      <c r="L8">
-        <v>8652032</v>
-      </c>
-      <c r="M8" t="s">
-        <v>38</v>
-      </c>
-      <c r="N8">
-        <v>1195</v>
-      </c>
-      <c r="O8">
-        <v>1287</v>
-      </c>
-      <c r="P8">
-        <v>1</v>
-      </c>
-      <c r="Q8">
-        <v>279</v>
-      </c>
-      <c r="R8">
-        <v>93</v>
-      </c>
-      <c r="S8">
-        <v>137</v>
-      </c>
-      <c r="T8">
-        <v>67.742000000000004</v>
-      </c>
-      <c r="U8">
-        <v>3.06</v>
-      </c>
-      <c r="V8">
-        <v>41</v>
-      </c>
-      <c r="W8">
+      <c r="S8" s="4">
+        <v>171</v>
+      </c>
+      <c r="T8" s="4">
+        <v>96.429000000000002</v>
+      </c>
+      <c r="U8" s="4">
+        <v>2.58</v>
+      </c>
+      <c r="V8" s="4">
+        <v>59</v>
+      </c>
+      <c r="W8" s="4">
         <v>0</v>
       </c>
-      <c r="X8">
+      <c r="X8" s="4">
         <v>0</v>
       </c>
-      <c r="Y8">
-        <v>282</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>79</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>28</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>29</v>
-      </c>
-      <c r="AC8" t="s">
-        <v>30</v>
-      </c>
-      <c r="AD8" t="s">
-        <v>80</v>
-      </c>
-      <c r="AE8" t="s">
-        <v>81</v>
+      <c r="Y8" s="4">
+        <v>255</v>
+      </c>
+      <c r="Z8" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA8" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB8" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC8" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD8" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE8" s="4" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="B9" t="s">
-        <v>65</v>
-      </c>
-      <c r="C9" s="4">
+      <c r="B9" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" s="5">
         <v>102</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="E9" t="s">
-        <v>66</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="D9" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G9" t="s">
-        <v>68</v>
-      </c>
-      <c r="H9" t="s">
-        <v>69</v>
-      </c>
-      <c r="I9" t="s">
-        <v>70</v>
-      </c>
-      <c r="J9" t="s">
+      <c r="G9" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="J9" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K9">
-        <v>8211</v>
-      </c>
-      <c r="L9">
-        <v>8465</v>
-      </c>
-      <c r="M9" t="s">
+      <c r="K9" s="4">
+        <v>3652</v>
+      </c>
+      <c r="L9" s="4">
+        <v>3945</v>
+      </c>
+      <c r="M9" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="N9">
-        <v>14</v>
-      </c>
-      <c r="O9">
+      <c r="N9" s="4">
+        <v>1</v>
+      </c>
+      <c r="O9" s="4">
         <v>97</v>
       </c>
-      <c r="P9">
+      <c r="P9" s="4">
         <v>1</v>
       </c>
-      <c r="Q9">
-        <v>252</v>
-      </c>
-      <c r="R9">
-        <v>84</v>
-      </c>
-      <c r="S9">
-        <v>171</v>
-      </c>
-      <c r="T9">
-        <v>96.429000000000002</v>
-      </c>
-      <c r="U9">
-        <v>2.58</v>
-      </c>
-      <c r="V9">
+      <c r="Q9" s="4">
+        <v>291</v>
+      </c>
+      <c r="R9" s="4">
+        <v>97</v>
+      </c>
+      <c r="S9" s="4">
+        <v>206</v>
+      </c>
+      <c r="T9" s="4">
+        <v>100</v>
+      </c>
+      <c r="U9" s="4">
+        <v>6.52</v>
+      </c>
+      <c r="V9" s="4">
+        <v>73</v>
+      </c>
+      <c r="W9" s="4">
+        <v>0</v>
+      </c>
+      <c r="X9" s="4">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="4">
+        <v>294</v>
+      </c>
+      <c r="Z9" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB9" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC9" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="W9">
-        <v>0</v>
-      </c>
-      <c r="X9">
-        <v>0</v>
-      </c>
-      <c r="Y9">
-        <v>255</v>
-      </c>
-      <c r="Z9" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA9" t="s">
-        <v>46</v>
-      </c>
-      <c r="AB9" t="s">
-        <v>58</v>
-      </c>
-      <c r="AC9" t="s">
-        <v>59</v>
-      </c>
-      <c r="AD9" t="s">
+      <c r="AD9" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="AE9" t="s">
-        <v>67</v>
+      <c r="AE9" s="4" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B10" t="s">
-        <v>65</v>
-      </c>
-      <c r="C10" s="4">
+      <c r="A10" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="C10" s="5">
+        <v>105</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="K10" s="4">
+        <v>8651751</v>
+      </c>
+      <c r="L10" s="4">
+        <v>8652032</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="N10" s="4">
+        <v>1195</v>
+      </c>
+      <c r="O10" s="4">
+        <v>1287</v>
+      </c>
+      <c r="P10" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="4">
+        <v>279</v>
+      </c>
+      <c r="R10" s="4">
         <v>93</v>
       </c>
-      <c r="E10" t="s">
-        <v>57</v>
-      </c>
-      <c r="F10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G10" t="s">
-        <v>62</v>
-      </c>
-      <c r="H10" t="s">
-        <v>63</v>
-      </c>
-      <c r="I10" t="s">
-        <v>64</v>
-      </c>
-      <c r="J10" t="s">
-        <v>37</v>
-      </c>
-      <c r="K10">
-        <v>3652</v>
-      </c>
-      <c r="L10">
-        <v>3945</v>
-      </c>
-      <c r="M10" t="s">
-        <v>38</v>
-      </c>
-      <c r="N10">
-        <v>1</v>
-      </c>
-      <c r="O10">
-        <v>97</v>
-      </c>
-      <c r="P10">
-        <v>1</v>
-      </c>
-      <c r="Q10">
-        <v>291</v>
-      </c>
-      <c r="R10">
-        <v>97</v>
-      </c>
-      <c r="S10">
-        <v>206</v>
-      </c>
-      <c r="T10">
-        <v>100</v>
-      </c>
-      <c r="U10">
-        <v>6.52</v>
-      </c>
-      <c r="V10">
-        <v>73</v>
-      </c>
-      <c r="W10">
+      <c r="S10" s="4">
+        <v>137</v>
+      </c>
+      <c r="T10" s="4">
+        <v>67.742000000000004</v>
+      </c>
+      <c r="U10" s="4">
+        <v>3.06</v>
+      </c>
+      <c r="V10" s="4">
+        <v>41</v>
+      </c>
+      <c r="W10" s="4">
         <v>0</v>
       </c>
-      <c r="X10">
+      <c r="X10" s="4">
         <v>0</v>
       </c>
-      <c r="Y10">
-        <v>294</v>
-      </c>
-      <c r="Z10" t="s">
-        <v>57</v>
-      </c>
-      <c r="AA10" t="s">
-        <v>46</v>
-      </c>
-      <c r="AB10" t="s">
-        <v>58</v>
-      </c>
-      <c r="AC10" t="s">
-        <v>59</v>
-      </c>
-      <c r="AD10" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE10" t="s">
-        <v>61</v>
+      <c r="Y10" s="4">
+        <v>282</v>
+      </c>
+      <c r="Z10" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD10" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE10" s="4" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AF10">
-    <sortCondition ref="B2:B10"/>
-    <sortCondition ref="F2:F10"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AE10">
+    <sortCondition ref="C2:C10"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>